<commit_message>
Day_7 | Git Links Added
</commit_message>
<xml_diff>
--- a/Batch/14/In_Class/Day_7.xlsx
+++ b/Batch/14/In_Class/Day_7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\14\In_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7920047-BA1D-4EAA-8E8F-4DE96F673776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B902B56C-3C4E-4D6A-81B2-6C3C9B3D4592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
+    <workbookView xWindow="-28920" yWindow="750" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3813" uniqueCount="348">
   <si>
     <t>Intro To excel</t>
   </si>
@@ -435,9 +435,6 @@
     <t>Data Validation</t>
   </si>
   <si>
-    <t>https://github.com/starlordali4444/Acciojob-Excel/blob/main/notes/Day7_Pivot_Tables.xlsx</t>
-  </si>
-  <si>
     <t>Date of Joining</t>
   </si>
   <si>
@@ -1081,6 +1078,12 @@
   </si>
   <si>
     <t>The customer support department wants to analyze which combination of job title, location, and years of experience has the highest average salary. How would you set this up?</t>
+  </si>
+  <si>
+    <t>https://github.com/starlordali4444/Acciojob-Excel/blob/master/Batch/14/Curriculum/Day_7_Pivot_Tables.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/starlordali4444/Acciojob-Excel/blob/master/Batch/14/Curriculum/Day_7_Data_validation.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1661,7 @@
         <v>68</v>
       </c>
       <c r="P1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
@@ -27556,8 +27559,8 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27577,7 +27580,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>131</v>
+        <v>346</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -27603,36 +27606,36 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" t="s">
         <v>235</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>236</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>237</v>
-      </c>
-      <c r="F6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -27642,17 +27645,17 @@
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -27665,12 +27668,12 @@
         <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -27689,6 +27692,14 @@
       <c r="B20" t="s">
         <v>130</v>
       </c>
+      <c r="C20" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -27696,6 +27707,12 @@
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -27707,14 +27724,16 @@
     <row r="24" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="25" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E3:J4"/>
+    <mergeCell ref="C20:H21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{28377F20-4E35-4015-87A7-928FE9847439}"/>
+    <hyperlink ref="C20" r:id="rId2" xr:uid="{51791E3E-E068-4CA3-9339-5CB4FF546330}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -27734,502 +27753,502 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B89" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B92" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B97" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B98" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B101" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -28242,7 +28261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A0040B-4877-432F-B0E4-47497118716B}">
   <dimension ref="B2:B141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R68" sqref="R68"/>
     </sheetView>
   </sheetViews>
@@ -28250,507 +28269,507 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B87" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B89" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B91" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B97" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B101" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B103" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B105" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B107" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B109" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B111" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B113" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B115" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B117" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B119" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B121" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B123" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B127" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B129" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B131" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B133" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B135" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B137" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B139" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B141" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>